<commit_message>
Refactor OracleTriggerAnalyzer and enhance logging for improved functionality
- Updated the OracleTriggerAnalyzer to read SQL content directly from a file path instead of passing the content as a string.
- Introduced a new method to append data to an existing Excel sheet, enhancing data management capabilities.
- Commented out the obsolete from_file class method for future reference.
- Improved logging throughout the OracleTriggerAnalyzer for better debugging visibility.
- Cleaned up whitespace and improved code readability across various files.
</commit_message>
<xml_diff>
--- a/utilities/oracle_postgresql_mappings.xlsx
+++ b/utilities/oracle_postgresql_mappings.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4545" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="data_type_mappings" sheetId="1" state="visible" r:id="rId1"/>
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -33,6 +33,17 @@
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <sz val="10.5"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -70,13 +81,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,10 +464,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.5703125" bestFit="1" customWidth="1" style="3" min="1" max="2"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="2" min="1" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="3">
+    <row r="1" ht="18.75" customHeight="1" s="2">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Oracle_Type</t>
@@ -465,7 +479,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1" s="3">
+    <row r="2" ht="18.75" customHeight="1" s="2">
       <c r="A2" t="inlineStr">
         <is>
           <t>varchar2</t>
@@ -477,7 +491,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1" s="3">
+    <row r="3" ht="18.75" customHeight="1" s="2">
       <c r="A3" t="inlineStr">
         <is>
           <t>nvarchar2</t>
@@ -489,7 +503,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="18.75" customHeight="1" s="3">
+    <row r="4" ht="18.75" customHeight="1" s="2">
       <c r="A4" t="inlineStr">
         <is>
           <t>nchar</t>
@@ -501,7 +515,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="18.75" customHeight="1" s="3">
+    <row r="5" ht="18.75" customHeight="1" s="2">
       <c r="A5" t="inlineStr">
         <is>
           <t>long</t>
@@ -513,7 +527,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="18.75" customHeight="1" s="3">
+    <row r="6" ht="18.75" customHeight="1" s="2">
       <c r="A6" t="inlineStr">
         <is>
           <t>rawid</t>
@@ -525,7 +539,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="18.75" customHeight="1" s="3">
+    <row r="7" ht="18.75" customHeight="1" s="2">
       <c r="A7" t="inlineStr">
         <is>
           <t>urowid</t>
@@ -537,7 +551,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="18.75" customHeight="1" s="3">
+    <row r="8" ht="18.75" customHeight="1" s="2">
       <c r="A8" t="inlineStr">
         <is>
           <t>number</t>
@@ -549,7 +563,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="18.75" customHeight="1" s="3">
+    <row r="9" ht="18.75" customHeight="1" s="2">
       <c r="A9" t="inlineStr">
         <is>
           <t>float</t>
@@ -561,7 +575,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="18.75" customHeight="1" s="3">
+    <row r="10" ht="18.75" customHeight="1" s="2">
       <c r="A10" t="inlineStr">
         <is>
           <t>binary_float</t>
@@ -573,7 +587,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="18.75" customHeight="1" s="3">
+    <row r="11" ht="18.75" customHeight="1" s="2">
       <c r="A11" t="inlineStr">
         <is>
           <t>binary_double</t>
@@ -585,7 +599,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="18.75" customHeight="1" s="3">
+    <row r="12" ht="18.75" customHeight="1" s="2">
       <c r="A12" t="inlineStr">
         <is>
           <t>pls_integer</t>
@@ -597,7 +611,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="18.75" customHeight="1" s="3">
+    <row r="13" ht="18.75" customHeight="1" s="2">
       <c r="A13" t="inlineStr">
         <is>
           <t>simple_integer</t>
@@ -609,7 +623,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="18.75" customHeight="1" s="3">
+    <row r="14" ht="18.75" customHeight="1" s="2">
       <c r="A14" t="inlineStr">
         <is>
           <t>binary_integer</t>
@@ -621,7 +635,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="18.75" customHeight="1" s="3">
+    <row r="15" ht="18.75" customHeight="1" s="2">
       <c r="A15" t="inlineStr">
         <is>
           <t>positive</t>
@@ -633,7 +647,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="18.75" customHeight="1" s="3">
+    <row r="16" ht="18.75" customHeight="1" s="2">
       <c r="A16" t="inlineStr">
         <is>
           <t>natural</t>
@@ -645,7 +659,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="18.75" customHeight="1" s="3">
+    <row r="17" ht="18.75" customHeight="1" s="2">
       <c r="A17" t="inlineStr">
         <is>
           <t>signtype</t>
@@ -657,7 +671,7 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="18.75" customHeight="1" s="3">
+    <row r="18" ht="18.75" customHeight="1" s="2">
       <c r="A18" t="inlineStr">
         <is>
           <t>smallint</t>
@@ -669,7 +683,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="18.75" customHeight="1" s="3">
+    <row r="19" ht="18.75" customHeight="1" s="2">
       <c r="A19" t="inlineStr">
         <is>
           <t>integer</t>
@@ -681,7 +695,7 @@
         </is>
       </c>
     </row>
-    <row r="20" ht="18.75" customHeight="1" s="3">
+    <row r="20" ht="18.75" customHeight="1" s="2">
       <c r="A20" t="inlineStr">
         <is>
           <t>int</t>
@@ -693,7 +707,7 @@
         </is>
       </c>
     </row>
-    <row r="21" ht="18.75" customHeight="1" s="3">
+    <row r="21" ht="18.75" customHeight="1" s="2">
       <c r="A21" t="inlineStr">
         <is>
           <t>decimal</t>
@@ -705,7 +719,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="18.75" customHeight="1" s="3">
+    <row r="22" ht="18.75" customHeight="1" s="2">
       <c r="A22" t="inlineStr">
         <is>
           <t>numeric</t>
@@ -717,7 +731,7 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="18.75" customHeight="1" s="3">
+    <row r="23" ht="18.75" customHeight="1" s="2">
       <c r="A23" t="inlineStr">
         <is>
           <t>real</t>
@@ -729,7 +743,7 @@
         </is>
       </c>
     </row>
-    <row r="24" ht="18.75" customHeight="1" s="3">
+    <row r="24" ht="18.75" customHeight="1" s="2">
       <c r="A24" t="inlineStr">
         <is>
           <t>date</t>
@@ -741,7 +755,7 @@
         </is>
       </c>
     </row>
-    <row r="25" ht="18.75" customHeight="1" s="3">
+    <row r="25" ht="18.75" customHeight="1" s="2">
       <c r="A25" t="inlineStr">
         <is>
           <t>timestamp with time zone</t>
@@ -753,7 +767,7 @@
         </is>
       </c>
     </row>
-    <row r="26" ht="18.75" customHeight="1" s="3">
+    <row r="26" ht="18.75" customHeight="1" s="2">
       <c r="A26" t="inlineStr">
         <is>
           <t>timestamp with local time zone</t>
@@ -765,7 +779,7 @@
         </is>
       </c>
     </row>
-    <row r="27" ht="18.75" customHeight="1" s="3">
+    <row r="27" ht="18.75" customHeight="1" s="2">
       <c r="A27" t="inlineStr">
         <is>
           <t>interval year to month</t>
@@ -777,7 +791,7 @@
         </is>
       </c>
     </row>
-    <row r="28" ht="18.75" customHeight="1" s="3">
+    <row r="28" ht="18.75" customHeight="1" s="2">
       <c r="A28" t="inlineStr">
         <is>
           <t>interval day to second</t>
@@ -789,7 +803,7 @@
         </is>
       </c>
     </row>
-    <row r="29" ht="18.75" customHeight="1" s="3">
+    <row r="29" ht="18.75" customHeight="1" s="2">
       <c r="A29" t="inlineStr">
         <is>
           <t>clob</t>
@@ -801,7 +815,7 @@
         </is>
       </c>
     </row>
-    <row r="30" ht="18.75" customHeight="1" s="3">
+    <row r="30" ht="18.75" customHeight="1" s="2">
       <c r="A30" t="inlineStr">
         <is>
           <t>nclob</t>
@@ -813,7 +827,7 @@
         </is>
       </c>
     </row>
-    <row r="31" ht="18.75" customHeight="1" s="3">
+    <row r="31" ht="18.75" customHeight="1" s="2">
       <c r="A31" t="inlineStr">
         <is>
           <t>blob</t>
@@ -825,7 +839,7 @@
         </is>
       </c>
     </row>
-    <row r="32" ht="18.75" customHeight="1" s="3">
+    <row r="32" ht="18.75" customHeight="1" s="2">
       <c r="A32" t="inlineStr">
         <is>
           <t>bfile</t>
@@ -837,7 +851,7 @@
         </is>
       </c>
     </row>
-    <row r="33" ht="18.75" customHeight="1" s="3">
+    <row r="33" ht="18.75" customHeight="1" s="2">
       <c r="A33" t="inlineStr">
         <is>
           <t>xmltype</t>
@@ -849,7 +863,7 @@
         </is>
       </c>
     </row>
-    <row r="34" ht="18.75" customHeight="1" s="3">
+    <row r="34" ht="18.75" customHeight="1" s="2">
       <c r="A34" t="inlineStr">
         <is>
           <t>sdo_geometry</t>
@@ -861,7 +875,7 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="18.75" customHeight="1" s="3">
+    <row r="35" ht="18.75" customHeight="1" s="2">
       <c r="A35" t="inlineStr">
         <is>
           <t>varray</t>
@@ -873,7 +887,7 @@
         </is>
       </c>
     </row>
-    <row r="36" ht="18.75" customHeight="1" s="3">
+    <row r="36" ht="18.75" customHeight="1" s="2">
       <c r="A36" t="inlineStr">
         <is>
           <t>nested table</t>
@@ -885,7 +899,7 @@
         </is>
       </c>
     </row>
-    <row r="37" ht="18.75" customHeight="1" s="3">
+    <row r="37" ht="18.75" customHeight="1" s="2">
       <c r="A37" t="inlineStr">
         <is>
           <t>raw</t>
@@ -897,7 +911,7 @@
         </is>
       </c>
     </row>
-    <row r="38" ht="18.75" customHeight="1" s="3">
+    <row r="38" ht="18.75" customHeight="1" s="2">
       <c r="A38" t="inlineStr">
         <is>
           <t>long raw</t>
@@ -909,7 +923,7 @@
         </is>
       </c>
     </row>
-    <row r="39" ht="18.75" customHeight="1" s="3">
+    <row r="39" ht="18.75" customHeight="1" s="2">
       <c r="A39" t="inlineStr">
         <is>
           <t>rowid</t>
@@ -921,7 +935,7 @@
         </is>
       </c>
     </row>
-    <row r="40" ht="18.75" customHeight="1" s="3">
+    <row r="40" ht="18.75" customHeight="1" s="2">
       <c r="A40" t="inlineStr">
         <is>
           <t>naturaln</t>
@@ -933,7 +947,7 @@
         </is>
       </c>
     </row>
-    <row r="41" ht="18.75" customHeight="1" s="3">
+    <row r="41" ht="18.75" customHeight="1" s="2">
       <c r="A41" t="inlineStr">
         <is>
           <t>positiven</t>
@@ -945,7 +959,7 @@
         </is>
       </c>
     </row>
-    <row r="42" ht="18.75" customHeight="1" s="3">
+    <row r="42" ht="18.75" customHeight="1" s="2">
       <c r="A42" t="inlineStr">
         <is>
           <t>simple_double</t>
@@ -957,7 +971,7 @@
         </is>
       </c>
     </row>
-    <row r="43" ht="18.75" customHeight="1" s="3">
+    <row r="43" ht="18.75" customHeight="1" s="2">
       <c r="A43" t="inlineStr">
         <is>
           <t>simple_float</t>
@@ -988,10 +1002,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.5703125" bestFit="1" customWidth="1" style="3" min="1" max="2"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="2" min="1" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="20.25" customHeight="1" s="3">
+    <row r="1" ht="20.25" customHeight="1" s="2">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Oracle_Function</t>
@@ -1003,7 +1017,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1" s="3">
+    <row r="2" ht="18.75" customHeight="1" s="2">
       <c r="A2" t="inlineStr">
         <is>
           <t>substr</t>
@@ -1015,7 +1029,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1" s="3">
+    <row r="3" ht="18.75" customHeight="1" s="2">
       <c r="A3" t="inlineStr">
         <is>
           <t>instr</t>
@@ -1027,7 +1041,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="18.75" customHeight="1" s="3">
+    <row r="4" ht="18.75" customHeight="1" s="2">
       <c r="A4" t="inlineStr">
         <is>
           <t>length</t>
@@ -1039,7 +1053,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="18.75" customHeight="1" s="3">
+    <row r="5" ht="18.75" customHeight="1" s="2">
       <c r="A5" t="inlineStr">
         <is>
           <t>trim</t>
@@ -1051,7 +1065,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="18.75" customHeight="1" s="3">
+    <row r="6" ht="18.75" customHeight="1" s="2">
       <c r="A6" t="inlineStr">
         <is>
           <t>ltrim</t>
@@ -1063,7 +1077,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="18.75" customHeight="1" s="3">
+    <row r="7" ht="18.75" customHeight="1" s="2">
       <c r="A7" t="inlineStr">
         <is>
           <t>rtrim</t>
@@ -1075,7 +1089,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="18.75" customHeight="1" s="3">
+    <row r="8" ht="18.75" customHeight="1" s="2">
       <c r="A8" t="inlineStr">
         <is>
           <t>upper</t>
@@ -1087,7 +1101,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="18.75" customHeight="1" s="3">
+    <row r="9" ht="18.75" customHeight="1" s="2">
       <c r="A9" t="inlineStr">
         <is>
           <t>lower</t>
@@ -1099,7 +1113,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="18.75" customHeight="1" s="3">
+    <row r="10" ht="18.75" customHeight="1" s="2">
       <c r="A10" t="inlineStr">
         <is>
           <t>initcap</t>
@@ -1111,7 +1125,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="18.75" customHeight="1" s="3">
+    <row r="11" ht="18.75" customHeight="1" s="2">
       <c r="A11" t="inlineStr">
         <is>
           <t>replace</t>
@@ -1123,7 +1137,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="18.75" customHeight="1" s="3">
+    <row r="12" ht="18.75" customHeight="1" s="2">
       <c r="A12" t="inlineStr">
         <is>
           <t>translate</t>
@@ -1135,7 +1149,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="18.75" customHeight="1" s="3">
+    <row r="13" ht="18.75" customHeight="1" s="2">
       <c r="A13" t="inlineStr">
         <is>
           <t>lpad</t>
@@ -1147,7 +1161,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="18.75" customHeight="1" s="3">
+    <row r="14" ht="18.75" customHeight="1" s="2">
       <c r="A14" t="inlineStr">
         <is>
           <t>rpad</t>
@@ -1159,7 +1173,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="18.75" customHeight="1" s="3">
+    <row r="15" ht="18.75" customHeight="1" s="2">
       <c r="A15" t="inlineStr">
         <is>
           <t>chr</t>
@@ -1171,7 +1185,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="18.75" customHeight="1" s="3">
+    <row r="16" ht="18.75" customHeight="1" s="2">
       <c r="A16" t="inlineStr">
         <is>
           <t>ascii</t>
@@ -1183,7 +1197,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="18.75" customHeight="1" s="3">
+    <row r="17" ht="18.75" customHeight="1" s="2">
       <c r="A17" t="inlineStr">
         <is>
           <t>concat</t>
@@ -1195,7 +1209,7 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="18.75" customHeight="1" s="3">
+    <row r="18" ht="18.75" customHeight="1" s="2">
       <c r="A18" t="inlineStr">
         <is>
           <t>reverse</t>
@@ -1207,7 +1221,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="18.75" customHeight="1" s="3">
+    <row r="19" ht="18.75" customHeight="1" s="2">
       <c r="A19" t="inlineStr">
         <is>
           <t>soundex</t>
@@ -1219,7 +1233,7 @@
         </is>
       </c>
     </row>
-    <row r="20" ht="18.75" customHeight="1" s="3">
+    <row r="20" ht="18.75" customHeight="1" s="2">
       <c r="A20" t="inlineStr">
         <is>
           <t>nvl</t>
@@ -1231,7 +1245,7 @@
         </is>
       </c>
     </row>
-    <row r="21" ht="18.75" customHeight="1" s="3">
+    <row r="21" ht="18.75" customHeight="1" s="2">
       <c r="A21" t="inlineStr">
         <is>
           <t>nvl2</t>
@@ -1243,7 +1257,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="18.75" customHeight="1" s="3">
+    <row r="22" ht="18.75" customHeight="1" s="2">
       <c r="A22" t="inlineStr">
         <is>
           <t>nullif</t>
@@ -1255,7 +1269,7 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="18.75" customHeight="1" s="3">
+    <row r="23" ht="18.75" customHeight="1" s="2">
       <c r="A23" t="inlineStr">
         <is>
           <t>decode</t>
@@ -1267,7 +1281,7 @@
         </is>
       </c>
     </row>
-    <row r="24" ht="18.75" customHeight="1" s="3">
+    <row r="24" ht="18.75" customHeight="1" s="2">
       <c r="A24" t="inlineStr">
         <is>
           <t>sysdate</t>
@@ -1279,7 +1293,7 @@
         </is>
       </c>
     </row>
-    <row r="25" ht="18.75" customHeight="1" s="3">
+    <row r="25" ht="18.75" customHeight="1" s="2">
       <c r="A25" t="inlineStr">
         <is>
           <t>current_date</t>
@@ -1291,7 +1305,7 @@
         </is>
       </c>
     </row>
-    <row r="26" ht="18.75" customHeight="1" s="3">
+    <row r="26" ht="18.75" customHeight="1" s="2">
       <c r="A26" t="inlineStr">
         <is>
           <t>current_timestamp</t>
@@ -1303,7 +1317,7 @@
         </is>
       </c>
     </row>
-    <row r="27" ht="18.75" customHeight="1" s="3">
+    <row r="27" ht="18.75" customHeight="1" s="2">
       <c r="A27" t="inlineStr">
         <is>
           <t>trunc</t>
@@ -1315,7 +1329,7 @@
         </is>
       </c>
     </row>
-    <row r="28" ht="18.75" customHeight="1" s="3">
+    <row r="28" ht="18.75" customHeight="1" s="2">
       <c r="A28" t="inlineStr">
         <is>
           <t>round</t>
@@ -1327,7 +1341,7 @@
         </is>
       </c>
     </row>
-    <row r="29" ht="18.75" customHeight="1" s="3">
+    <row r="29" ht="18.75" customHeight="1" s="2">
       <c r="A29" t="inlineStr">
         <is>
           <t>to_date</t>
@@ -1339,7 +1353,7 @@
         </is>
       </c>
     </row>
-    <row r="30" ht="18.75" customHeight="1" s="3">
+    <row r="30" ht="18.75" customHeight="1" s="2">
       <c r="A30" t="inlineStr">
         <is>
           <t>to_char</t>
@@ -1351,7 +1365,7 @@
         </is>
       </c>
     </row>
-    <row r="31" ht="18.75" customHeight="1" s="3">
+    <row r="31" ht="18.75" customHeight="1" s="2">
       <c r="A31" t="inlineStr">
         <is>
           <t>extract</t>
@@ -1363,7 +1377,7 @@
         </is>
       </c>
     </row>
-    <row r="32" ht="18.75" customHeight="1" s="3">
+    <row r="32" ht="18.75" customHeight="1" s="2">
       <c r="A32" t="inlineStr">
         <is>
           <t>add_months</t>
@@ -1375,7 +1389,7 @@
         </is>
       </c>
     </row>
-    <row r="33" ht="18.75" customHeight="1" s="3">
+    <row r="33" ht="18.75" customHeight="1" s="2">
       <c r="A33" t="inlineStr">
         <is>
           <t>months_between</t>
@@ -1387,7 +1401,7 @@
         </is>
       </c>
     </row>
-    <row r="34" ht="18.75" customHeight="1" s="3">
+    <row r="34" ht="18.75" customHeight="1" s="2">
       <c r="A34" t="inlineStr">
         <is>
           <t>next_day</t>
@@ -1399,7 +1413,7 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="18.75" customHeight="1" s="3">
+    <row r="35" ht="18.75" customHeight="1" s="2">
       <c r="A35" t="inlineStr">
         <is>
           <t>last_day</t>
@@ -1411,7 +1425,7 @@
         </is>
       </c>
     </row>
-    <row r="36" ht="18.75" customHeight="1" s="3">
+    <row r="36" ht="18.75" customHeight="1" s="2">
       <c r="A36" t="inlineStr">
         <is>
           <t>dateadd</t>
@@ -1423,7 +1437,7 @@
         </is>
       </c>
     </row>
-    <row r="37" ht="18.75" customHeight="1" s="3">
+    <row r="37" ht="18.75" customHeight="1" s="2">
       <c r="A37" t="inlineStr">
         <is>
           <t>datediff</t>
@@ -1435,7 +1449,7 @@
         </is>
       </c>
     </row>
-    <row r="38" ht="18.75" customHeight="1" s="3">
+    <row r="38" ht="18.75" customHeight="1" s="2">
       <c r="A38" t="inlineStr">
         <is>
           <t>abs</t>
@@ -1447,7 +1461,7 @@
         </is>
       </c>
     </row>
-    <row r="39" ht="18.75" customHeight="1" s="3">
+    <row r="39" ht="18.75" customHeight="1" s="2">
       <c r="A39" t="inlineStr">
         <is>
           <t>ceil</t>
@@ -1459,7 +1473,7 @@
         </is>
       </c>
     </row>
-    <row r="40" ht="18.75" customHeight="1" s="3">
+    <row r="40" ht="18.75" customHeight="1" s="2">
       <c r="A40" t="inlineStr">
         <is>
           <t>floor</t>
@@ -1471,7 +1485,7 @@
         </is>
       </c>
     </row>
-    <row r="41" ht="18.75" customHeight="1" s="3">
+    <row r="41" ht="18.75" customHeight="1" s="2">
       <c r="A41" t="inlineStr">
         <is>
           <t>mod</t>
@@ -1483,7 +1497,7 @@
         </is>
       </c>
     </row>
-    <row r="42" ht="18.75" customHeight="1" s="3">
+    <row r="42" ht="18.75" customHeight="1" s="2">
       <c r="A42" t="inlineStr">
         <is>
           <t>power</t>
@@ -1495,7 +1509,7 @@
         </is>
       </c>
     </row>
-    <row r="43" ht="18.75" customHeight="1" s="3">
+    <row r="43" ht="18.75" customHeight="1" s="2">
       <c r="A43" t="inlineStr">
         <is>
           <t>sqrt</t>
@@ -1507,7 +1521,7 @@
         </is>
       </c>
     </row>
-    <row r="44" ht="18.75" customHeight="1" s="3">
+    <row r="44" ht="18.75" customHeight="1" s="2">
       <c r="A44" t="inlineStr">
         <is>
           <t>exp</t>
@@ -1519,7 +1533,7 @@
         </is>
       </c>
     </row>
-    <row r="45" ht="18.75" customHeight="1" s="3">
+    <row r="45" ht="18.75" customHeight="1" s="2">
       <c r="A45" t="inlineStr">
         <is>
           <t>ln</t>
@@ -1531,7 +1545,7 @@
         </is>
       </c>
     </row>
-    <row r="46" ht="18.75" customHeight="1" s="3">
+    <row r="46" ht="18.75" customHeight="1" s="2">
       <c r="A46" t="inlineStr">
         <is>
           <t>log</t>
@@ -1543,7 +1557,7 @@
         </is>
       </c>
     </row>
-    <row r="47" ht="18.75" customHeight="1" s="3">
+    <row r="47" ht="18.75" customHeight="1" s="2">
       <c r="A47" t="inlineStr">
         <is>
           <t>sin</t>
@@ -1555,7 +1569,7 @@
         </is>
       </c>
     </row>
-    <row r="48" ht="18.75" customHeight="1" s="3">
+    <row r="48" ht="18.75" customHeight="1" s="2">
       <c r="A48" t="inlineStr">
         <is>
           <t>cos</t>
@@ -1567,7 +1581,7 @@
         </is>
       </c>
     </row>
-    <row r="49" ht="18.75" customHeight="1" s="3">
+    <row r="49" ht="18.75" customHeight="1" s="2">
       <c r="A49" t="inlineStr">
         <is>
           <t>tan</t>
@@ -1579,7 +1593,7 @@
         </is>
       </c>
     </row>
-    <row r="50" ht="18.75" customHeight="1" s="3">
+    <row r="50" ht="18.75" customHeight="1" s="2">
       <c r="A50" t="inlineStr">
         <is>
           <t>asin</t>
@@ -1591,7 +1605,7 @@
         </is>
       </c>
     </row>
-    <row r="51" ht="18.75" customHeight="1" s="3">
+    <row r="51" ht="18.75" customHeight="1" s="2">
       <c r="A51" t="inlineStr">
         <is>
           <t>acos</t>
@@ -1603,7 +1617,7 @@
         </is>
       </c>
     </row>
-    <row r="52" ht="18.75" customHeight="1" s="3">
+    <row r="52" ht="18.75" customHeight="1" s="2">
       <c r="A52" t="inlineStr">
         <is>
           <t>atan</t>
@@ -1615,7 +1629,7 @@
         </is>
       </c>
     </row>
-    <row r="53" ht="18.75" customHeight="1" s="3">
+    <row r="53" ht="18.75" customHeight="1" s="2">
       <c r="A53" t="inlineStr">
         <is>
           <t>atan2</t>
@@ -1627,7 +1641,7 @@
         </is>
       </c>
     </row>
-    <row r="54" ht="18.75" customHeight="1" s="3">
+    <row r="54" ht="18.75" customHeight="1" s="2">
       <c r="A54" t="inlineStr">
         <is>
           <t>sinh</t>
@@ -1639,7 +1653,7 @@
         </is>
       </c>
     </row>
-    <row r="55" ht="18.75" customHeight="1" s="3">
+    <row r="55" ht="18.75" customHeight="1" s="2">
       <c r="A55" t="inlineStr">
         <is>
           <t>cosh</t>
@@ -1651,7 +1665,7 @@
         </is>
       </c>
     </row>
-    <row r="56" ht="18.75" customHeight="1" s="3">
+    <row r="56" ht="18.75" customHeight="1" s="2">
       <c r="A56" t="inlineStr">
         <is>
           <t>tanh</t>
@@ -1663,7 +1677,7 @@
         </is>
       </c>
     </row>
-    <row r="57" ht="18.75" customHeight="1" s="3">
+    <row r="57" ht="18.75" customHeight="1" s="2">
       <c r="A57" t="inlineStr">
         <is>
           <t>sign</t>
@@ -1675,7 +1689,7 @@
         </is>
       </c>
     </row>
-    <row r="58" ht="18.75" customHeight="1" s="3">
+    <row r="58" ht="18.75" customHeight="1" s="2">
       <c r="A58" t="inlineStr">
         <is>
           <t>to_number</t>
@@ -1687,7 +1701,7 @@
         </is>
       </c>
     </row>
-    <row r="59" ht="18.75" customHeight="1" s="3">
+    <row r="59" ht="18.75" customHeight="1" s="2">
       <c r="A59" t="inlineStr">
         <is>
           <t>count</t>
@@ -1699,7 +1713,7 @@
         </is>
       </c>
     </row>
-    <row r="60" ht="18.75" customHeight="1" s="3">
+    <row r="60" ht="18.75" customHeight="1" s="2">
       <c r="A60" t="inlineStr">
         <is>
           <t>sum</t>
@@ -1711,7 +1725,7 @@
         </is>
       </c>
     </row>
-    <row r="61" ht="18.75" customHeight="1" s="3">
+    <row r="61" ht="18.75" customHeight="1" s="2">
       <c r="A61" t="inlineStr">
         <is>
           <t>avg</t>
@@ -1723,7 +1737,7 @@
         </is>
       </c>
     </row>
-    <row r="62" ht="18.75" customHeight="1" s="3">
+    <row r="62" ht="18.75" customHeight="1" s="2">
       <c r="A62" t="inlineStr">
         <is>
           <t>min</t>
@@ -1735,7 +1749,7 @@
         </is>
       </c>
     </row>
-    <row r="63" ht="18.75" customHeight="1" s="3">
+    <row r="63" ht="18.75" customHeight="1" s="2">
       <c r="A63" t="inlineStr">
         <is>
           <t>max</t>
@@ -1747,7 +1761,7 @@
         </is>
       </c>
     </row>
-    <row r="64" ht="18.75" customHeight="1" s="3">
+    <row r="64" ht="18.75" customHeight="1" s="2">
       <c r="A64" t="inlineStr">
         <is>
           <t>stddev</t>
@@ -1759,7 +1773,7 @@
         </is>
       </c>
     </row>
-    <row r="65" ht="18.75" customHeight="1" s="3">
+    <row r="65" ht="18.75" customHeight="1" s="2">
       <c r="A65" t="inlineStr">
         <is>
           <t>variance</t>
@@ -1771,7 +1785,7 @@
         </is>
       </c>
     </row>
-    <row r="66" ht="18.75" customHeight="1" s="3">
+    <row r="66" ht="18.75" customHeight="1" s="2">
       <c r="A66" t="inlineStr">
         <is>
           <t>median</t>
@@ -1783,7 +1797,7 @@
         </is>
       </c>
     </row>
-    <row r="67" ht="18.75" customHeight="1" s="3">
+    <row r="67" ht="18.75" customHeight="1" s="2">
       <c r="A67" t="inlineStr">
         <is>
           <t>listagg</t>
@@ -1795,7 +1809,7 @@
         </is>
       </c>
     </row>
-    <row r="68" ht="18.75" customHeight="1" s="3">
+    <row r="68" ht="18.75" customHeight="1" s="2">
       <c r="A68" t="inlineStr">
         <is>
           <t>wm_concat</t>
@@ -1807,7 +1821,7 @@
         </is>
       </c>
     </row>
-    <row r="69" ht="18.75" customHeight="1" s="3">
+    <row r="69" ht="18.75" customHeight="1" s="2">
       <c r="A69" t="inlineStr">
         <is>
           <t>row_number</t>
@@ -1819,7 +1833,7 @@
         </is>
       </c>
     </row>
-    <row r="70" ht="18.75" customHeight="1" s="3">
+    <row r="70" ht="18.75" customHeight="1" s="2">
       <c r="A70" t="inlineStr">
         <is>
           <t>rank</t>
@@ -1831,7 +1845,7 @@
         </is>
       </c>
     </row>
-    <row r="71" ht="18.75" customHeight="1" s="3">
+    <row r="71" ht="18.75" customHeight="1" s="2">
       <c r="A71" t="inlineStr">
         <is>
           <t>dense_rank</t>
@@ -1843,7 +1857,7 @@
         </is>
       </c>
     </row>
-    <row r="72" ht="18.75" customHeight="1" s="3">
+    <row r="72" ht="18.75" customHeight="1" s="2">
       <c r="A72" t="inlineStr">
         <is>
           <t>first_value</t>
@@ -1855,7 +1869,7 @@
         </is>
       </c>
     </row>
-    <row r="73" ht="18.75" customHeight="1" s="3">
+    <row r="73" ht="18.75" customHeight="1" s="2">
       <c r="A73" t="inlineStr">
         <is>
           <t>last_value</t>
@@ -1867,7 +1881,7 @@
         </is>
       </c>
     </row>
-    <row r="74" ht="18.75" customHeight="1" s="3">
+    <row r="74" ht="18.75" customHeight="1" s="2">
       <c r="A74" t="inlineStr">
         <is>
           <t>lead</t>
@@ -1879,7 +1893,7 @@
         </is>
       </c>
     </row>
-    <row r="75" ht="18.75" customHeight="1" s="3">
+    <row r="75" ht="18.75" customHeight="1" s="2">
       <c r="A75" t="inlineStr">
         <is>
           <t>lag</t>
@@ -1891,7 +1905,7 @@
         </is>
       </c>
     </row>
-    <row r="76" ht="18.75" customHeight="1" s="3">
+    <row r="76" ht="18.75" customHeight="1" s="2">
       <c r="A76" t="inlineStr">
         <is>
           <t>ntile</t>
@@ -1903,7 +1917,7 @@
         </is>
       </c>
     </row>
-    <row r="77" ht="18.75" customHeight="1" s="3">
+    <row r="77" ht="18.75" customHeight="1" s="2">
       <c r="A77" t="inlineStr">
         <is>
           <t>percent_rank</t>
@@ -1915,7 +1929,7 @@
         </is>
       </c>
     </row>
-    <row r="78" ht="18.75" customHeight="1" s="3">
+    <row r="78" ht="18.75" customHeight="1" s="2">
       <c r="A78" t="inlineStr">
         <is>
           <t>cume_dist</t>
@@ -1927,7 +1941,7 @@
         </is>
       </c>
     </row>
-    <row r="79" ht="18.75" customHeight="1" s="3">
+    <row r="79" ht="18.75" customHeight="1" s="2">
       <c r="A79" t="inlineStr">
         <is>
           <t>cast</t>
@@ -1939,7 +1953,7 @@
         </is>
       </c>
     </row>
-    <row r="80" ht="18.75" customHeight="1" s="3">
+    <row r="80" ht="18.75" customHeight="1" s="2">
       <c r="A80" t="inlineStr">
         <is>
           <t>convert</t>
@@ -1951,7 +1965,7 @@
         </is>
       </c>
     </row>
-    <row r="81" ht="18.75" customHeight="1" s="3">
+    <row r="81" ht="18.75" customHeight="1" s="2">
       <c r="A81" t="inlineStr">
         <is>
           <t>hextoraw</t>
@@ -1963,7 +1977,7 @@
         </is>
       </c>
     </row>
-    <row r="82" ht="18.75" customHeight="1" s="3">
+    <row r="82" ht="18.75" customHeight="1" s="2">
       <c r="A82" t="inlineStr">
         <is>
           <t>rawtohex</t>
@@ -1975,7 +1989,7 @@
         </is>
       </c>
     </row>
-    <row r="83" ht="18.75" customHeight="1" s="3">
+    <row r="83" ht="18.75" customHeight="1" s="2">
       <c r="A83" t="inlineStr">
         <is>
           <t>user</t>
@@ -1987,7 +2001,7 @@
         </is>
       </c>
     </row>
-    <row r="84" ht="18.75" customHeight="1" s="3">
+    <row r="84" ht="18.75" customHeight="1" s="2">
       <c r="A84" t="inlineStr">
         <is>
           <t>uid</t>
@@ -1999,7 +2013,7 @@
         </is>
       </c>
     </row>
-    <row r="85" ht="18.75" customHeight="1" s="3">
+    <row r="85" ht="18.75" customHeight="1" s="2">
       <c r="A85" t="inlineStr">
         <is>
           <t>userenv</t>
@@ -2011,7 +2025,7 @@
         </is>
       </c>
     </row>
-    <row r="86" ht="18.75" customHeight="1" s="3">
+    <row r="86" ht="18.75" customHeight="1" s="2">
       <c r="A86" t="inlineStr">
         <is>
           <t>sys_context</t>
@@ -2023,7 +2037,7 @@
         </is>
       </c>
     </row>
-    <row r="87" ht="18.75" customHeight="1" s="3">
+    <row r="87" ht="18.75" customHeight="1" s="2">
       <c r="A87" t="inlineStr">
         <is>
           <t>sys_guid</t>
@@ -2035,7 +2049,7 @@
         </is>
       </c>
     </row>
-    <row r="88" ht="18.75" customHeight="1" s="3">
+    <row r="88" ht="18.75" customHeight="1" s="2">
       <c r="A88" t="inlineStr">
         <is>
           <t>sessiontimezone</t>
@@ -2047,7 +2061,7 @@
         </is>
       </c>
     </row>
-    <row r="89" ht="18.75" customHeight="1" s="3">
+    <row r="89" ht="18.75" customHeight="1" s="2">
       <c r="A89" t="inlineStr">
         <is>
           <t>dbtimezone</t>
@@ -2059,7 +2073,7 @@
         </is>
       </c>
     </row>
-    <row r="90" ht="18.75" customHeight="1" s="3">
+    <row r="90" ht="18.75" customHeight="1" s="2">
       <c r="A90" t="inlineStr">
         <is>
           <t>nextval</t>
@@ -2071,7 +2085,7 @@
         </is>
       </c>
     </row>
-    <row r="91" ht="18.75" customHeight="1" s="3">
+    <row r="91" ht="18.75" customHeight="1" s="2">
       <c r="A91" t="inlineStr">
         <is>
           <t>currval</t>
@@ -2083,7 +2097,7 @@
         </is>
       </c>
     </row>
-    <row r="92" ht="18.75" customHeight="1" s="3">
+    <row r="92" ht="18.75" customHeight="1" s="2">
       <c r="A92" t="inlineStr">
         <is>
           <t>empty_clob</t>
@@ -2095,7 +2109,7 @@
         </is>
       </c>
     </row>
-    <row r="93" ht="18.75" customHeight="1" s="3">
+    <row r="93" ht="18.75" customHeight="1" s="2">
       <c r="A93" t="inlineStr">
         <is>
           <t>empty_blob</t>
@@ -2107,7 +2121,7 @@
         </is>
       </c>
     </row>
-    <row r="94" ht="18.75" customHeight="1" s="3">
+    <row r="94" ht="18.75" customHeight="1" s="2">
       <c r="A94" t="inlineStr">
         <is>
           <t>dbms_lob.getlength</t>
@@ -2119,7 +2133,7 @@
         </is>
       </c>
     </row>
-    <row r="95" ht="18.75" customHeight="1" s="3">
+    <row r="95" ht="18.75" customHeight="1" s="2">
       <c r="A95" t="inlineStr">
         <is>
           <t>dbms_lob.substr</t>
@@ -2131,7 +2145,7 @@
         </is>
       </c>
     </row>
-    <row r="96" ht="18.75" customHeight="1" s="3">
+    <row r="96" ht="18.75" customHeight="1" s="2">
       <c r="A96" t="inlineStr">
         <is>
           <t>vsize</t>
@@ -2143,7 +2157,7 @@
         </is>
       </c>
     </row>
-    <row r="97" ht="18.75" customHeight="1" s="3">
+    <row r="97" ht="18.75" customHeight="1" s="2">
       <c r="A97" t="inlineStr">
         <is>
           <t>dump</t>
@@ -2155,7 +2169,7 @@
         </is>
       </c>
     </row>
-    <row r="98" ht="18.75" customHeight="1" s="3">
+    <row r="98" ht="18.75" customHeight="1" s="2">
       <c r="A98" t="inlineStr">
         <is>
           <t>greatest</t>
@@ -2167,7 +2181,7 @@
         </is>
       </c>
     </row>
-    <row r="99" ht="18.75" customHeight="1" s="3">
+    <row r="99" ht="18.75" customHeight="1" s="2">
       <c r="A99" t="inlineStr">
         <is>
           <t>least</t>
@@ -2179,7 +2193,7 @@
         </is>
       </c>
     </row>
-    <row r="100" ht="18.75" customHeight="1" s="3">
+    <row r="100" ht="18.75" customHeight="1" s="2">
       <c r="A100" t="inlineStr">
         <is>
           <t>regexp_like</t>
@@ -2191,7 +2205,7 @@
         </is>
       </c>
     </row>
-    <row r="101" ht="18.75" customHeight="1" s="3">
+    <row r="101" ht="18.75" customHeight="1" s="2">
       <c r="A101" t="inlineStr">
         <is>
           <t>regexp_replace</t>
@@ -2203,7 +2217,7 @@
         </is>
       </c>
     </row>
-    <row r="102" ht="18.75" customHeight="1" s="3">
+    <row r="102" ht="18.75" customHeight="1" s="2">
       <c r="A102" t="inlineStr">
         <is>
           <t>regexp_substr</t>
@@ -2215,7 +2229,7 @@
         </is>
       </c>
     </row>
-    <row r="103" ht="18.75" customHeight="1" s="3">
+    <row r="103" ht="18.75" customHeight="1" s="2">
       <c r="A103" t="inlineStr">
         <is>
           <t>regexp_instr</t>
@@ -2227,7 +2241,7 @@
         </is>
       </c>
     </row>
-    <row r="104" ht="18.75" customHeight="1" s="3">
+    <row r="104" ht="18.75" customHeight="1" s="2">
       <c r="A104" t="inlineStr">
         <is>
           <t>regexp_count</t>
@@ -2239,28 +2253,28 @@
         </is>
       </c>
     </row>
-    <row r="105" ht="18.75" customHeight="1" s="3">
+    <row r="105" ht="18.75" customHeight="1" s="2">
       <c r="A105" t="inlineStr">
         <is>
           <t>connect_by_root</t>
         </is>
       </c>
     </row>
-    <row r="106" ht="18.75" customHeight="1" s="3">
+    <row r="106" ht="18.75" customHeight="1" s="2">
       <c r="A106" t="inlineStr">
         <is>
           <t>sys_connect_by_path</t>
         </is>
       </c>
     </row>
-    <row r="107" ht="18.75" customHeight="1" s="3">
+    <row r="107" ht="18.75" customHeight="1" s="2">
       <c r="A107" t="inlineStr">
         <is>
           <t>level</t>
         </is>
       </c>
     </row>
-    <row r="108" ht="18.75" customHeight="1" s="3">
+    <row r="108" ht="18.75" customHeight="1" s="2">
       <c r="A108" t="inlineStr">
         <is>
           <t>xmltype</t>
@@ -2272,7 +2286,7 @@
         </is>
       </c>
     </row>
-    <row r="109" ht="18.75" customHeight="1" s="3">
+    <row r="109" ht="18.75" customHeight="1" s="2">
       <c r="A109" t="inlineStr">
         <is>
           <t>extractvalue</t>
@@ -2284,7 +2298,7 @@
         </is>
       </c>
     </row>
-    <row r="110" ht="18.75" customHeight="1" s="3">
+    <row r="110" ht="18.75" customHeight="1" s="2">
       <c r="A110" t="inlineStr">
         <is>
           <t>xmlserialize</t>
@@ -2296,7 +2310,7 @@
         </is>
       </c>
     </row>
-    <row r="111" ht="18.75" customHeight="1" s="3">
+    <row r="111" ht="18.75" customHeight="1" s="2">
       <c r="A111" t="inlineStr">
         <is>
           <t>xmlquery</t>
@@ -2308,7 +2322,7 @@
         </is>
       </c>
     </row>
-    <row r="112" ht="18.75" customHeight="1" s="3">
+    <row r="112" ht="18.75" customHeight="1" s="2">
       <c r="A112" t="inlineStr">
         <is>
           <t>json_value</t>
@@ -2320,7 +2334,7 @@
         </is>
       </c>
     </row>
-    <row r="113" ht="18.75" customHeight="1" s="3">
+    <row r="113" ht="18.75" customHeight="1" s="2">
       <c r="A113" t="inlineStr">
         <is>
           <t>json_query</t>
@@ -2332,7 +2346,7 @@
         </is>
       </c>
     </row>
-    <row r="114" ht="18.75" customHeight="1" s="3">
+    <row r="114" ht="18.75" customHeight="1" s="2">
       <c r="A114" t="inlineStr">
         <is>
           <t>json_table</t>
@@ -2344,7 +2358,7 @@
         </is>
       </c>
     </row>
-    <row r="115" ht="18.75" customHeight="1" s="3">
+    <row r="115" ht="18.75" customHeight="1" s="2">
       <c r="A115" t="inlineStr">
         <is>
           <t>is_json</t>
@@ -2356,7 +2370,7 @@
         </is>
       </c>
     </row>
-    <row r="116" ht="18.75" customHeight="1" s="3">
+    <row r="116" ht="18.75" customHeight="1" s="2">
       <c r="A116" t="inlineStr">
         <is>
           <t>sqlcode</t>
@@ -2368,7 +2382,7 @@
         </is>
       </c>
     </row>
-    <row r="117" ht="18.75" customHeight="1" s="3">
+    <row r="117" ht="18.75" customHeight="1" s="2">
       <c r="A117" t="inlineStr">
         <is>
           <t>sqlerrm</t>
@@ -2391,15 +2405,40 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col width="10.140625" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
+    <col width="4.42578125" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
+    <col width="7.7109375" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
+    <col width="9.140625" customWidth="1" style="4" min="4" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>filename</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>line</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>line_no</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
 
@@ -2411,7 +2450,7 @@
   </sheetPr>
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -2528,10 +2567,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.5703125" bestFit="1" customWidth="1" style="3" min="1" max="2"/>
+    <col width="13.5703125" bestFit="1" customWidth="1" style="2" min="1" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1" s="3">
+    <row r="1" ht="18.75" customHeight="1" s="2">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Oracle_Exception</t>
@@ -2543,7 +2582,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="18.75" customHeight="1" s="3">
+    <row r="2" ht="18.75" customHeight="1" s="2">
       <c r="A2" t="inlineStr">
         <is>
           <t>invalid_theme_no</t>
@@ -2555,7 +2594,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="18.75" customHeight="1" s="3">
+    <row r="3" ht="18.75" customHeight="1" s="2">
       <c r="A3" t="inlineStr">
         <is>
           <t>delete_no_more_possible</t>
@@ -2567,7 +2606,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="18.75" customHeight="1" s="3">
+    <row r="4" ht="18.75" customHeight="1" s="2">
       <c r="A4" t="inlineStr">
         <is>
           <t>theme_no_only_insert</t>
@@ -2579,7 +2618,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="18.75" customHeight="1" s="3">
+    <row r="5" ht="18.75" customHeight="1" s="2">
       <c r="A5" t="inlineStr">
         <is>
           <t>description_too_long</t>
@@ -2591,7 +2630,7 @@
         </is>
       </c>
     </row>
-    <row r="6" ht="18.75" customHeight="1" s="3">
+    <row r="6" ht="18.75" customHeight="1" s="2">
       <c r="A6" t="inlineStr">
         <is>
           <t>theme_desc_proposal_too_long</t>
@@ -2603,7 +2642,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="18.75" customHeight="1" s="3">
+    <row r="7" ht="18.75" customHeight="1" s="2">
       <c r="A7" t="inlineStr">
         <is>
           <t>theme_desc_alt_too_long</t>
@@ -2615,7 +2654,7 @@
         </is>
       </c>
     </row>
-    <row r="8" ht="18.75" customHeight="1" s="3">
+    <row r="8" ht="18.75" customHeight="1" s="2">
       <c r="A8" t="inlineStr">
         <is>
           <t>theme_no_cannot_be_inserted</t>
@@ -2627,7 +2666,7 @@
         </is>
       </c>
     </row>
-    <row r="9" ht="18.75" customHeight="1" s="3">
+    <row r="9" ht="18.75" customHeight="1" s="2">
       <c r="A9" t="inlineStr">
         <is>
           <t>onlyoneofficialchangeperday</t>
@@ -2639,7 +2678,7 @@
         </is>
       </c>
     </row>
-    <row r="10" ht="18.75" customHeight="1" s="3">
+    <row r="10" ht="18.75" customHeight="1" s="2">
       <c r="A10" t="inlineStr">
         <is>
           <t>insertsmustbeofficial</t>
@@ -2651,7 +2690,7 @@
         </is>
       </c>
     </row>
-    <row r="11" ht="18.75" customHeight="1" s="3">
+    <row r="11" ht="18.75" customHeight="1" s="2">
       <c r="A11" t="inlineStr">
         <is>
           <t>themedescriptionmandatory</t>
@@ -2663,7 +2702,7 @@
         </is>
       </c>
     </row>
-    <row r="12" ht="18.75" customHeight="1" s="3">
+    <row r="12" ht="18.75" customHeight="1" s="2">
       <c r="A12" t="inlineStr">
         <is>
           <t>theme_desc_not_unique</t>
@@ -2675,7 +2714,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="18.75" customHeight="1" s="3">
+    <row r="13" ht="18.75" customHeight="1" s="2">
       <c r="A13" t="inlineStr">
         <is>
           <t>in_prep_not_portf_proj</t>
@@ -2687,7 +2726,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="18.75" customHeight="1" s="3">
+    <row r="14" ht="18.75" customHeight="1" s="2">
       <c r="A14" t="inlineStr">
         <is>
           <t>in_prep_not_closed</t>
@@ -2699,7 +2738,7 @@
         </is>
       </c>
     </row>
-    <row r="15" ht="18.75" customHeight="1" s="3">
+    <row r="15" ht="18.75" customHeight="1" s="2">
       <c r="A15" t="inlineStr">
         <is>
           <t>invalid_molecule_id</t>
@@ -2711,7 +2750,7 @@
         </is>
       </c>
     </row>
-    <row r="16" ht="18.75" customHeight="1" s="3">
+    <row r="16" ht="18.75" customHeight="1" s="2">
       <c r="A16" t="inlineStr">
         <is>
           <t>sec_mol_list_not_empty</t>
@@ -2723,7 +2762,7 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="18.75" customHeight="1" s="3">
+    <row r="17" ht="18.75" customHeight="1" s="2">
       <c r="A17" t="inlineStr">
         <is>
           <t>admin_update_only</t>
@@ -2735,7 +2774,7 @@
         </is>
       </c>
     </row>
-    <row r="18" ht="18.75" customHeight="1" s="3">
+    <row r="18" ht="18.75" customHeight="1" s="2">
       <c r="A18" t="inlineStr">
         <is>
           <t>portf_proj_mol_cre_err</t>
@@ -2747,7 +2786,7 @@
         </is>
       </c>
     </row>
-    <row r="19" ht="18.75" customHeight="1" s="3">
+    <row r="19" ht="18.75" customHeight="1" s="2">
       <c r="A19" t="inlineStr">
         <is>
           <t>debugging</t>
@@ -2759,7 +2798,7 @@
         </is>
       </c>
     </row>
-    <row r="20" ht="18.75" customHeight="1" s="3">
+    <row r="20" ht="18.75" customHeight="1" s="2">
       <c r="A20" t="inlineStr">
         <is>
           <t>err_map_exists</t>
@@ -2771,7 +2810,7 @@
         </is>
       </c>
     </row>
-    <row r="21" ht="18.75" customHeight="1" s="3">
+    <row r="21" ht="18.75" customHeight="1" s="2">
       <c r="A21" t="inlineStr">
         <is>
           <t>err_molec_id_missing</t>
@@ -2783,7 +2822,7 @@
         </is>
       </c>
     </row>
-    <row r="22" ht="18.75" customHeight="1" s="3">
+    <row r="22" ht="18.75" customHeight="1" s="2">
       <c r="A22" t="inlineStr">
         <is>
           <t>err_no_portf_molecule_left</t>
@@ -2795,7 +2834,7 @@
         </is>
       </c>
     </row>
-    <row r="23" ht="18.75" customHeight="1" s="3">
+    <row r="23" ht="18.75" customHeight="1" s="2">
       <c r="A23" t="inlineStr">
         <is>
           <t>err_upd_inv_map</t>
@@ -2807,7 +2846,7 @@
         </is>
       </c>
     </row>
-    <row r="24" ht="18.75" customHeight="1" s="3">
+    <row r="24" ht="18.75" customHeight="1" s="2">
       <c r="A24" t="inlineStr">
         <is>
           <t>err_ins_inv_map</t>
@@ -2819,7 +2858,7 @@
         </is>
       </c>
     </row>
-    <row r="25" ht="18.75" customHeight="1" s="3">
+    <row r="25" ht="18.75" customHeight="1" s="2">
       <c r="A25" t="inlineStr">
         <is>
           <t>err_inv_mol_sequence</t>
@@ -2831,7 +2870,7 @@
         </is>
       </c>
     </row>
-    <row r="26" ht="18.75" customHeight="1" s="3">
+    <row r="26" ht="18.75" customHeight="1" s="2">
       <c r="A26" t="inlineStr">
         <is>
           <t>update_upd</t>
@@ -2843,7 +2882,7 @@
         </is>
       </c>
     </row>
-    <row r="27" ht="18.75" customHeight="1" s="3">
+    <row r="27" ht="18.75" customHeight="1" s="2">
       <c r="A27" t="inlineStr">
         <is>
           <t>err_upd</t>
@@ -2855,7 +2894,7 @@
         </is>
       </c>
     </row>
-    <row r="28" ht="18.75" customHeight="1" s="3">
+    <row r="28" ht="18.75" customHeight="1" s="2">
       <c r="A28" t="inlineStr">
         <is>
           <t>err_ins</t>
@@ -2867,7 +2906,7 @@
         </is>
       </c>
     </row>
-    <row r="29" ht="18.75" customHeight="1" s="3">
+    <row r="29" ht="18.75" customHeight="1" s="2">
       <c r="A29" t="inlineStr">
         <is>
           <t>err_ctry_chg</t>
@@ -2879,7 +2918,7 @@
         </is>
       </c>
     </row>
-    <row r="30" ht="18.75" customHeight="1" s="3">
+    <row r="30" ht="18.75" customHeight="1" s="2">
       <c r="A30" t="inlineStr">
         <is>
           <t>err_not_allowed_to_invalidate</t>
@@ -2891,7 +2930,7 @@
         </is>
       </c>
     </row>
-    <row r="31" ht="18.75" customHeight="1" s="3">
+    <row r="31" ht="18.75" customHeight="1" s="2">
       <c r="A31" t="inlineStr">
         <is>
           <t>test_err</t>
@@ -2903,7 +2942,7 @@
         </is>
       </c>
     </row>
-    <row r="32" ht="18.75" customHeight="1" s="3">
+    <row r="32" ht="18.75" customHeight="1" s="2">
       <c r="A32" t="inlineStr">
         <is>
           <t>err_ins_legal_addr</t>
@@ -2915,7 +2954,7 @@
         </is>
       </c>
     </row>
-    <row r="33" ht="18.75" customHeight="1" s="3">
+    <row r="33" ht="18.75" customHeight="1" s="2">
       <c r="A33" t="inlineStr">
         <is>
           <t>no_data_found</t>
@@ -2927,7 +2966,7 @@
         </is>
       </c>
     </row>
-    <row r="34" ht="18.75" customHeight="1" s="3">
+    <row r="34" ht="18.75" customHeight="1" s="2">
       <c r="A34" t="inlineStr">
         <is>
           <t>too_many_rows</t>
@@ -2939,7 +2978,7 @@
         </is>
       </c>
     </row>
-    <row r="35" ht="18.75" customHeight="1" s="3">
+    <row r="35" ht="18.75" customHeight="1" s="2">
       <c r="A35" t="inlineStr">
         <is>
           <t>dup_val_on_index</t>
@@ -2951,7 +2990,7 @@
         </is>
       </c>
     </row>
-    <row r="36" ht="18.75" customHeight="1" s="3">
+    <row r="36" ht="18.75" customHeight="1" s="2">
       <c r="A36" t="inlineStr">
         <is>
           <t>value_error</t>
@@ -2963,7 +3002,7 @@
         </is>
       </c>
     </row>
-    <row r="37" ht="18.75" customHeight="1" s="3">
+    <row r="37" ht="18.75" customHeight="1" s="2">
       <c r="A37" t="inlineStr">
         <is>
           <t>invalid_number</t>
@@ -2975,7 +3014,7 @@
         </is>
       </c>
     </row>
-    <row r="38" ht="18.75" customHeight="1" s="3">
+    <row r="38" ht="18.75" customHeight="1" s="2">
       <c r="A38" t="inlineStr">
         <is>
           <t>zero_divide</t>
@@ -2987,7 +3026,7 @@
         </is>
       </c>
     </row>
-    <row r="39" ht="18.75" customHeight="1" s="3">
+    <row r="39" ht="18.75" customHeight="1" s="2">
       <c r="A39" t="inlineStr">
         <is>
           <t>invalid_cursor</t>
@@ -2999,7 +3038,7 @@
         </is>
       </c>
     </row>
-    <row r="40" ht="18.75" customHeight="1" s="3">
+    <row r="40" ht="18.75" customHeight="1" s="2">
       <c r="A40" t="inlineStr">
         <is>
           <t>cursor_already_open</t>
@@ -3011,7 +3050,7 @@
         </is>
       </c>
     </row>
-    <row r="41" ht="18.75" customHeight="1" s="3">
+    <row r="41" ht="18.75" customHeight="1" s="2">
       <c r="A41" t="inlineStr">
         <is>
           <t>not_logged_on</t>
@@ -3023,7 +3062,7 @@
         </is>
       </c>
     </row>
-    <row r="42" ht="18.75" customHeight="1" s="3">
+    <row r="42" ht="18.75" customHeight="1" s="2">
       <c r="A42" t="inlineStr">
         <is>
           <t>login_denied</t>
@@ -3035,7 +3074,7 @@
         </is>
       </c>
     </row>
-    <row r="43" ht="18.75" customHeight="1" s="3">
+    <row r="43" ht="18.75" customHeight="1" s="2">
       <c r="A43" t="inlineStr">
         <is>
           <t>program_error</t>
@@ -3047,7 +3086,7 @@
         </is>
       </c>
     </row>
-    <row r="44" ht="18.75" customHeight="1" s="3">
+    <row r="44" ht="18.75" customHeight="1" s="2">
       <c r="A44" t="inlineStr">
         <is>
           <t>storage_error</t>
@@ -3059,7 +3098,7 @@
         </is>
       </c>
     </row>
-    <row r="45" ht="18.75" customHeight="1" s="3">
+    <row r="45" ht="18.75" customHeight="1" s="2">
       <c r="A45" t="inlineStr">
         <is>
           <t>timeout_on_resource</t>
@@ -3071,7 +3110,7 @@
         </is>
       </c>
     </row>
-    <row r="46" ht="18.75" customHeight="1" s="3">
+    <row r="46" ht="18.75" customHeight="1" s="2">
       <c r="A46" t="inlineStr">
         <is>
           <t>invalid_rowid</t>
@@ -3083,7 +3122,7 @@
         </is>
       </c>
     </row>
-    <row r="47" ht="18.75" customHeight="1" s="3">
+    <row r="47" ht="18.75" customHeight="1" s="2">
       <c r="A47" t="inlineStr">
         <is>
           <t>rowtype_mismatch</t>
@@ -3095,7 +3134,7 @@
         </is>
       </c>
     </row>
-    <row r="48" ht="18.75" customHeight="1" s="3">
+    <row r="48" ht="18.75" customHeight="1" s="2">
       <c r="A48" t="inlineStr">
         <is>
           <t>self_is_null</t>
@@ -3107,7 +3146,7 @@
         </is>
       </c>
     </row>
-    <row r="49" ht="18.75" customHeight="1" s="3">
+    <row r="49" ht="18.75" customHeight="1" s="2">
       <c r="A49" t="inlineStr">
         <is>
           <t>subscript_outside_limit</t>
@@ -3119,7 +3158,7 @@
         </is>
       </c>
     </row>
-    <row r="50" ht="18.75" customHeight="1" s="3">
+    <row r="50" ht="18.75" customHeight="1" s="2">
       <c r="A50" t="inlineStr">
         <is>
           <t>subscript_beyond_count</t>
@@ -3131,7 +3170,7 @@
         </is>
       </c>
     </row>
-    <row r="51" ht="18.75" customHeight="1" s="3">
+    <row r="51" ht="18.75" customHeight="1" s="2">
       <c r="A51" t="inlineStr">
         <is>
           <t>access_into_null</t>
@@ -3143,7 +3182,7 @@
         </is>
       </c>
     </row>
-    <row r="52" ht="18.75" customHeight="1" s="3">
+    <row r="52" ht="18.75" customHeight="1" s="2">
       <c r="A52" t="inlineStr">
         <is>
           <t>collection_is_null</t>
@@ -3155,7 +3194,7 @@
         </is>
       </c>
     </row>
-    <row r="53" ht="18.75" customHeight="1" s="3">
+    <row r="53" ht="18.75" customHeight="1" s="2">
       <c r="A53" t="inlineStr">
         <is>
           <t>others</t>

</xml_diff>

<commit_message>
Enhance logging and clean up code in main.py and utilities
- Updated logging in main.py to replace print statements with logger.debug for better debugging visibility.
- Cleaned up and organized code in various utility files, including FormatSQL and OracleTriggerAnalyzer, to improve readability and maintainability.
- Removed obsolete Excel handling function from common.py to streamline the codebase.
- Adjusted SQL exception handling in the OracleTriggerAnalyzer to use RAISE EXCEPTION for better error management.
- Updated parse timestamps in JSON files for accurate tracking.
</commit_message>
<xml_diff>
--- a/utilities/oracle_postgresql_mappings.xlsx
+++ b/utilities/oracle_postgresql_mappings.xlsx
@@ -9,21 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12315" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="data_type_mappings" sheetId="1" r:id="rId1"/>
     <sheet name="function_mappings" sheetId="2" r:id="rId2"/>
-    <sheet name="non_parse" sheetId="3" r:id="rId3"/>
-    <sheet name="function_list" sheetId="4" r:id="rId4"/>
-    <sheet name="exception_mappings" sheetId="5" r:id="rId5"/>
+    <sheet name="function_list" sheetId="4" r:id="rId3"/>
+    <sheet name="exception_mappings" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="388">
   <si>
     <t>Oracle_Type</t>
   </si>
@@ -826,15 +825,6 @@
     <t>SQLERRM</t>
   </si>
   <si>
-    <t>filename</t>
-  </si>
-  <si>
-    <t>line</t>
-  </si>
-  <si>
-    <t>line_no</t>
-  </si>
-  <si>
     <t>function_name</t>
   </si>
   <si>
@@ -874,6 +864,12 @@
     <t>GMD.GMD_UTIL_THEMES$UPD_THEME_DESC_JOB_PROC</t>
   </si>
   <si>
+    <t>mdm_util_internat_names.send_all_changes_notification</t>
+  </si>
+  <si>
+    <t>mdm_util_gtin.gtin_action</t>
+  </si>
+  <si>
     <t>Oracle_Exception</t>
   </si>
   <si>
@@ -1190,12 +1186,6 @@
   </si>
   <si>
     <t>Unknown error occurred</t>
-  </si>
-  <si>
-    <t>mdm_util_internat_names.send_all_changes_notification</t>
-  </si>
-  <si>
-    <t>mdm_util_gtin.gtin_action</t>
   </si>
 </sst>
 </file>
@@ -2884,134 +2874,101 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="65.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="C1" s="4" t="s">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>269</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="65.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>390</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -3027,426 +2984,426 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>283</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B2" t="s">
         <v>285</v>
-      </c>
-      <c r="B2" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B3" t="s">
         <v>287</v>
-      </c>
-      <c r="B3" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>288</v>
+      </c>
+      <c r="B4" t="s">
         <v>289</v>
-      </c>
-      <c r="B4" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>290</v>
+      </c>
+      <c r="B5" t="s">
         <v>291</v>
-      </c>
-      <c r="B5" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>292</v>
+      </c>
+      <c r="B6" t="s">
         <v>293</v>
-      </c>
-      <c r="B6" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B7" t="s">
         <v>295</v>
-      </c>
-      <c r="B7" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B8" t="s">
         <v>297</v>
-      </c>
-      <c r="B8" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>298</v>
+      </c>
+      <c r="B9" t="s">
         <v>299</v>
-      </c>
-      <c r="B9" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>300</v>
+      </c>
+      <c r="B10" t="s">
         <v>301</v>
-      </c>
-      <c r="B10" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>302</v>
+      </c>
+      <c r="B11" t="s">
         <v>303</v>
-      </c>
-      <c r="B11" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>304</v>
+      </c>
+      <c r="B12" t="s">
         <v>305</v>
-      </c>
-      <c r="B12" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>306</v>
+      </c>
+      <c r="B13" t="s">
         <v>307</v>
-      </c>
-      <c r="B13" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>308</v>
+      </c>
+      <c r="B14" t="s">
         <v>309</v>
-      </c>
-      <c r="B14" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>310</v>
+      </c>
+      <c r="B15" t="s">
         <v>311</v>
-      </c>
-      <c r="B15" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>312</v>
+      </c>
+      <c r="B16" t="s">
         <v>313</v>
-      </c>
-      <c r="B16" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>314</v>
+      </c>
+      <c r="B17" t="s">
         <v>315</v>
-      </c>
-      <c r="B17" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>316</v>
+      </c>
+      <c r="B18" t="s">
         <v>317</v>
-      </c>
-      <c r="B18" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B19" t="s">
         <v>319</v>
-      </c>
-      <c r="B19" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>320</v>
+      </c>
+      <c r="B20" t="s">
         <v>321</v>
-      </c>
-      <c r="B20" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>322</v>
+      </c>
+      <c r="B21" t="s">
         <v>323</v>
-      </c>
-      <c r="B21" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>324</v>
+      </c>
+      <c r="B22" t="s">
         <v>325</v>
-      </c>
-      <c r="B22" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>326</v>
+      </c>
+      <c r="B23" t="s">
         <v>327</v>
-      </c>
-      <c r="B23" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>328</v>
+      </c>
+      <c r="B24" t="s">
         <v>329</v>
-      </c>
-      <c r="B24" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>330</v>
+      </c>
+      <c r="B25" t="s">
         <v>331</v>
-      </c>
-      <c r="B25" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>332</v>
+      </c>
+      <c r="B26" t="s">
         <v>333</v>
-      </c>
-      <c r="B26" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>334</v>
+      </c>
+      <c r="B27" t="s">
         <v>335</v>
-      </c>
-      <c r="B27" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>336</v>
+      </c>
+      <c r="B28" t="s">
         <v>337</v>
-      </c>
-      <c r="B28" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>338</v>
+      </c>
+      <c r="B29" t="s">
         <v>339</v>
-      </c>
-      <c r="B29" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>340</v>
+      </c>
+      <c r="B30" t="s">
         <v>341</v>
-      </c>
-      <c r="B30" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>342</v>
+      </c>
+      <c r="B31" t="s">
         <v>343</v>
-      </c>
-      <c r="B31" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>344</v>
+      </c>
+      <c r="B32" t="s">
         <v>345</v>
-      </c>
-      <c r="B32" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>346</v>
+      </c>
+      <c r="B33" t="s">
         <v>347</v>
-      </c>
-      <c r="B33" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>348</v>
+      </c>
+      <c r="B34" t="s">
         <v>349</v>
-      </c>
-      <c r="B34" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>350</v>
+      </c>
+      <c r="B35" t="s">
         <v>351</v>
-      </c>
-      <c r="B35" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>352</v>
+      </c>
+      <c r="B36" t="s">
         <v>353</v>
-      </c>
-      <c r="B36" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>354</v>
+      </c>
+      <c r="B37" t="s">
         <v>355</v>
-      </c>
-      <c r="B37" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>356</v>
+      </c>
+      <c r="B38" t="s">
         <v>357</v>
-      </c>
-      <c r="B38" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>358</v>
+      </c>
+      <c r="B39" t="s">
         <v>359</v>
-      </c>
-      <c r="B39" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>360</v>
+      </c>
+      <c r="B40" t="s">
         <v>361</v>
-      </c>
-      <c r="B40" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>362</v>
+      </c>
+      <c r="B41" t="s">
         <v>363</v>
-      </c>
-      <c r="B41" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>364</v>
+      </c>
+      <c r="B42" t="s">
         <v>365</v>
-      </c>
-      <c r="B42" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>366</v>
+      </c>
+      <c r="B43" t="s">
         <v>367</v>
-      </c>
-      <c r="B43" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>368</v>
+      </c>
+      <c r="B44" t="s">
         <v>369</v>
-      </c>
-      <c r="B44" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>370</v>
+      </c>
+      <c r="B45" t="s">
         <v>371</v>
-      </c>
-      <c r="B45" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>372</v>
+      </c>
+      <c r="B46" t="s">
         <v>373</v>
-      </c>
-      <c r="B46" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>374</v>
+      </c>
+      <c r="B47" t="s">
         <v>375</v>
-      </c>
-      <c r="B47" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>376</v>
+      </c>
+      <c r="B48" t="s">
         <v>377</v>
-      </c>
-      <c r="B48" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>378</v>
+      </c>
+      <c r="B49" t="s">
         <v>379</v>
-      </c>
-      <c r="B49" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>380</v>
+      </c>
+      <c r="B50" t="s">
         <v>381</v>
-      </c>
-      <c r="B50" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>382</v>
+      </c>
+      <c r="B51" t="s">
         <v>383</v>
-      </c>
-      <c r="B51" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>384</v>
+      </c>
+      <c r="B52" t="s">
         <v>385</v>
-      </c>
-      <c r="B52" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>386</v>
+      </c>
+      <c r="B53" t="s">
         <v>387</v>
-      </c>
-      <c r="B53" t="s">
-        <v>388</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhance statement mapping functionality and improve OracleTriggerAnalyzer
- Added new statement mappings to the configuration page for better user guidance on SQL statement types.
- Implemented dynamic loading of statement mappings from an Excel file in the OracleTriggerAnalyzer to streamline conversion processes.
- Refactored the initialization of conversion statistics to incorporate loaded statement mappings, enhancing flexibility and maintainability.
- Updated the ConfigManager to include validation for unique statement entries in the Excel sheet, improving data integrity.
</commit_message>
<xml_diff>
--- a/utilities/oracle_postgresql_mappings.xlsx
+++ b/utilities/oracle_postgresql_mappings.xlsx
@@ -12,6 +12,7 @@
     <sheet name="exception_mappings" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="schema_mappings" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="function_mappings" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="statement_mappings" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2753,4 +2754,119 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>statement</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>statement_type</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SELECT</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>select_statement</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>INSERT</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>insert_statement</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>UPDATE</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>update_statement</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DELETE</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>delete_statement</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>RAISE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>raise_statement</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NULL </t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>null_statement</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>return_statement</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update OracleTriggerAnalyzer and mappings for improved exception handling and structure
- Refactored the OracleTriggerAnalyzer to enhance exception name tracking and mapping to PostgreSQL equivalents.
- Cleaned up unnecessary comments and improved code readability throughout the class.
- Updated the oracle_postgresql_mappings.xlsx to reflect new mappings and ensure accurate conversion processes.
- Enhanced logging for better visibility during exception handling and SQL parsing.
</commit_message>
<xml_diff>
--- a/utilities/oracle_postgresql_mappings.xlsx
+++ b/utilities/oracle_postgresql_mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DELOITTE\ORACALE_to_json\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F4910C-006D-408F-BBE2-A7064F57F9DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C62E65-7ABD-4BC5-B0BF-D4EDE354F2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_type_mappings" sheetId="1" r:id="rId1"/>
@@ -1174,7 +1174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1183,7 +1183,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2840,14 +2839,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3056,8 +3055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>